<commit_message>
updated the wait time
</commit_message>
<xml_diff>
--- a/TestDataAndResults/TestData/SophieAutomation.xlsx
+++ b/TestDataAndResults/TestData/SophieAutomation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C34059-38F0-43D4-B031-F407D3C6D4E3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03F603E-EBE2-42CB-979E-FAB9C3F0A1AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="292">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1753,8 +1753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2760,10 +2760,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3119,20 +3119,22 @@
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="C18" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="9">
+        <v>7000</v>
+      </c>
+      <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8">
@@ -3140,20 +3142,18 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>131</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="9"/>
     </row>
@@ -3162,19 +3162,19 @@
         <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="9"/>
@@ -3184,18 +3184,20 @@
         <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="1"/>
+        <v>75</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="G21" s="1"/>
       <c r="H21" s="9"/>
     </row>
@@ -3204,20 +3206,18 @@
         <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F22" s="1">
-        <v>3000</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="9"/>
     </row>
@@ -3226,18 +3226,20 @@
         <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>132</v>
+        <v>44</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3000</v>
+      </c>
       <c r="G23" s="1"/>
       <c r="H23" s="9"/>
     </row>
@@ -3246,19 +3248,19 @@
         <v>16</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
       <c r="H24" s="9"/>
     </row>
     <row r="25" spans="1:8">
@@ -3266,16 +3268,16 @@
         <v>16</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
@@ -3289,13 +3291,13 @@
         <v>96</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>93</v>
+        <v>135</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -3306,13 +3308,13 @@
         <v>16</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>287</v>
+        <v>136</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>93</v>
@@ -3326,13 +3328,13 @@
         <v>16</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>136</v>
+        <v>287</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>93</v>
@@ -3346,13 +3348,13 @@
         <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>93</v>
@@ -3366,15 +3368,15 @@
         <v>16</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="E30" s="20" t="s">
+      <c r="D30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F30" s="9"/>
@@ -3386,16 +3388,16 @@
         <v>16</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>49</v>
+        <v>136</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
@@ -3406,21 +3408,19 @@
         <v>16</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>44</v>
+        <v>137</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="1">
-        <v>3000</v>
-      </c>
-      <c r="G32" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
       <c r="H32" s="9"/>
     </row>
     <row r="33" spans="1:8">
@@ -3428,19 +3428,21 @@
         <v>16</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>137</v>
+        <v>44</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="F33" s="1">
+        <v>3000</v>
+      </c>
+      <c r="G33" s="1"/>
       <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8">
@@ -3448,13 +3450,13 @@
         <v>16</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>49</v>
@@ -3468,20 +3470,18 @@
         <v>16</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>142</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
     </row>
@@ -3490,13 +3490,13 @@
         <v>16</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>140</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>75</v>
@@ -3512,21 +3512,21 @@
         <v>16</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F37" s="13">
-        <v>43525</v>
-      </c>
-      <c r="G37" s="13"/>
+      <c r="F37" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="G37" s="9"/>
       <c r="H37" s="9"/>
     </row>
     <row r="38" spans="1:8">
@@ -3534,19 +3534,19 @@
         <v>16</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F38" s="13">
-        <v>45743</v>
+        <v>43525</v>
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="9"/>
@@ -3556,19 +3556,21 @@
         <v>16</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
+        <v>75</v>
+      </c>
+      <c r="F39" s="13">
+        <v>45743</v>
+      </c>
+      <c r="G39" s="13"/>
       <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8">
@@ -3579,10 +3581,10 @@
         <v>117</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>49</v>
@@ -3596,21 +3598,19 @@
         <v>16</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G41" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
       <c r="H41" s="9"/>
     </row>
     <row r="42" spans="1:8">
@@ -3621,15 +3621,17 @@
         <v>121</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F42" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="G42" s="1"/>
       <c r="H42" s="9"/>
     </row>
@@ -3638,20 +3640,18 @@
         <v>16</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>160</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="9"/>
     </row>
@@ -3660,19 +3660,21 @@
         <v>16</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
+        <v>154</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G44" s="1"/>
       <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8">
@@ -3686,14 +3688,12 @@
         <v>162</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F45" s="9">
-        <v>5000</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
     </row>
@@ -3702,18 +3702,20 @@
         <v>16</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>162</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>83</v>
+        <v>38</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F46" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="F46" s="9">
+        <v>5000</v>
+      </c>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
     </row>
@@ -3722,20 +3724,18 @@
         <v>16</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>44</v>
+        <v>162</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="9">
-        <v>10000</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F47" s="9"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
     </row>
@@ -3744,18 +3744,20 @@
         <v>16</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>103</v>
+        <v>44</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F48" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="F48" s="9">
+        <v>10000</v>
+      </c>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
     </row>
@@ -3767,10 +3769,10 @@
         <v>165</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>166</v>
+        <v>103</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>49</v>
@@ -3784,22 +3786,20 @@
         <v>16</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>108</v>
+        <v>165</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>44</v>
+        <v>166</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="1">
-        <v>20000</v>
-      </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
@@ -3809,15 +3809,17 @@
         <v>108</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="D51" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="F51" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" s="1">
+        <v>20000</v>
+      </c>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
@@ -3826,16 +3828,16 @@
         <v>16</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>112</v>
+        <v>290</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -3846,16 +3848,16 @@
         <v>16</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -3866,13 +3868,13 @@
         <v>16</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>116</v>
@@ -3889,17 +3891,15 @@
         <v>117</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F55" s="1">
-        <v>10000</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
     </row>
@@ -3908,18 +3908,20 @@
         <v>16</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F56" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F56" s="1">
+        <v>10000</v>
+      </c>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
     </row>
@@ -3928,16 +3930,16 @@
         <v>16</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>126</v>
+        <v>38</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -3948,20 +3950,18 @@
         <v>16</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F58" s="1">
-        <v>30000</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
     </row>
@@ -3970,20 +3970,42 @@
         <v>16</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>129</v>
+        <v>44</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F59" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="F59" s="1">
+        <v>30000</v>
+      </c>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="A60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4000,7 +4022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
@@ -5113,8 +5135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5585,7 +5607,7 @@
         <v>45</v>
       </c>
       <c r="F23" s="1">
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>

</xml_diff>

<commit_message>
check in for 3 scenarios
</commit_message>
<xml_diff>
--- a/TestDataAndResults/TestData/SophieAutomation.xlsx
+++ b/TestDataAndResults/TestData/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B927F24-CFDE-48F9-B2D6-201966EAF61E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204B1757-A26F-43DF-9CE7-3C4AB55A345B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1490" uniqueCount="291">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -806,9 +806,6 @@
     <t>Switch to child</t>
   </si>
   <si>
-    <t>bottom</t>
-  </si>
-  <si>
     <t>select the ProcessRTSpineDataMaster</t>
   </si>
   <si>
@@ -824,9 +821,6 @@
     <t>btnStart</t>
   </si>
   <si>
-    <t>top</t>
-  </si>
-  <si>
     <t>select the UpdateRTSpineDataChild</t>
   </si>
   <si>
@@ -903,6 +897,15 @@
   </si>
   <si>
     <t>free_mobile1</t>
+  </si>
+  <si>
+    <t>switchToFrameByIndex</t>
+  </si>
+  <si>
+    <t>switch to first frame</t>
+  </si>
+  <si>
+    <t>frame switch</t>
   </si>
 </sst>
 </file>
@@ -912,7 +915,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -952,6 +955,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibiri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1087,7 +1096,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1114,6 +1123,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1620,22 +1631,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="14.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="14.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" s="3" customFormat="1" ht="14.25">
       <c r="A3" s="4"/>
@@ -1767,38 +1778,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
@@ -2360,10 +2371,10 @@
         <v>97</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>92</v>
@@ -2571,10 +2582,10 @@
         <v>43</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -2797,38 +2808,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
@@ -3350,7 +3361,7 @@
         <v>97</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>94</v>
@@ -3413,7 +3424,7 @@
         <v>135</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>92</v>
@@ -3850,13 +3861,13 @@
         <v>107</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -3870,7 +3881,7 @@
         <v>107</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D53" s="20" t="s">
         <v>37</v>
@@ -4080,38 +4091,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
@@ -4634,7 +4645,7 @@
         <v>90</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>92</v>
@@ -4784,7 +4795,7 @@
         <v>170</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -4988,10 +4999,10 @@
         <v>43</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -5214,36 +5225,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
@@ -5872,7 +5883,7 @@
         <v>90</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>92</v>
@@ -6460,10 +6471,10 @@
         <v>43</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E61" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -6632,10 +6643,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6652,36 +6663,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="27"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
@@ -7388,20 +7399,18 @@
         <v>25</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>257</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
@@ -7410,18 +7419,20 @@
         <v>25</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>259</v>
+        <v>37</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="F38" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2</v>
+      </c>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
@@ -7433,15 +7444,17 @@
         <v>45</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>262</v>
+        <v>37</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F39" s="1"/>
+        <v>288</v>
+      </c>
+      <c r="F39" s="1">
+        <v>1</v>
+      </c>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
@@ -7450,16 +7463,16 @@
         <v>25</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>37</v>
+        <v>258</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>189</v>
+        <v>259</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -7470,20 +7483,18 @@
         <v>25</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>37</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>263</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
@@ -7492,20 +7503,166 @@
         <v>25</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F45" s="1">
+        <v>1</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E42" s="1" t="s">
+      <c r="C46" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F48" s="25">
+        <v>0</v>
+      </c>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
+      <c r="D49" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -7513,6 +7670,7 @@
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A3:H3"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -7522,8 +7680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7540,55 +7698,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29" t="s">
-        <v>266</v>
-      </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31" t="s">
+        <v>264</v>
+      </c>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>270</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -7598,16 +7756,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="E5" s="18" t="s">
         <v>272</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -7615,16 +7773,16 @@
         <v>0</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C6" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>272</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>276</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -7632,16 +7790,16 @@
         <v>16</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C7" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>272</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>277</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -7649,16 +7807,16 @@
         <v>16</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C8" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>272</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>273</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -7666,16 +7824,16 @@
         <v>16</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>141</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -7683,16 +7841,16 @@
         <v>22</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -7700,16 +7858,16 @@
         <v>22</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -7743,7 +7901,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -7751,7 +7909,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed the wait time
</commit_message>
<xml_diff>
--- a/TestDataAndResults/TestData/SophieAutomation.xlsx
+++ b/TestDataAndResults/TestData/SophieAutomation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8465869D-7ED0-4759-9F3D-4EF6F3D0E872}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A53B6C4-0B64-4EE5-9F4F-510FBA75D9BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2555,8 +2555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92316FED-85B2-43F2-9827-12AFBA752185}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16:F16"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3275,7 +3275,7 @@
         <v>41</v>
       </c>
       <c r="F35" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="9"/>
@@ -3317,7 +3317,7 @@
         <v>41</v>
       </c>
       <c r="F37" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="9"/>
@@ -3359,7 +3359,7 @@
         <v>41</v>
       </c>
       <c r="F39" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="9"/>
@@ -3401,7 +3401,7 @@
         <v>41</v>
       </c>
       <c r="F41" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="9"/>
@@ -3547,8 +3547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDE53E4-1746-48CE-AB4D-617AE971D39B}">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4266,7 +4266,7 @@
         <v>41</v>
       </c>
       <c r="F35" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="9"/>
@@ -4308,7 +4308,7 @@
         <v>41</v>
       </c>
       <c r="F37" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="9"/>
@@ -4350,7 +4350,7 @@
         <v>41</v>
       </c>
       <c r="F39" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G39" s="1"/>
       <c r="H39" s="9"/>
@@ -4392,7 +4392,7 @@
         <v>41</v>
       </c>
       <c r="F41" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G41" s="1"/>
       <c r="H41" s="9"/>
@@ -4872,8 +4872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B88A9-98DC-469F-B6A8-72D4BD0DF47F}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView topLeftCell="C70" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85:E85"/>
+    <sheetView topLeftCell="C76" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6388,7 +6388,7 @@
         <v>41</v>
       </c>
       <c r="F73" s="1">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G73" s="25"/>
       <c r="H73" s="25"/>
@@ -6430,7 +6430,7 @@
         <v>41</v>
       </c>
       <c r="F75" s="1">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G75" s="25"/>
       <c r="H75" s="25"/>
@@ -6520,7 +6520,7 @@
         <v>41</v>
       </c>
       <c r="F79" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G79" s="25"/>
       <c r="H79" s="25"/>
@@ -6562,7 +6562,7 @@
         <v>41</v>
       </c>
       <c r="F81" s="25">
-        <v>3000</v>
+        <v>7000</v>
       </c>
       <c r="G81" s="25"/>
       <c r="H81" s="25"/>
@@ -6662,8 +6662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353D209F-F23A-4BBD-9C0E-30D3275A1C3F}">
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B103" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
+      <selection activeCell="H99" sqref="H99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8746,7 +8746,7 @@
         <v>41</v>
       </c>
       <c r="F100" s="1">
-        <v>5000</v>
+        <v>15000</v>
       </c>
       <c r="G100" s="25"/>
       <c r="H100" s="25"/>
@@ -12840,7 +12840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
check in 71819 to run first scenario
</commit_message>
<xml_diff>
--- a/TestDataAndResults/TestData/SophieAutomation.xlsx
+++ b/TestDataAndResults/TestData/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A53B6C4-0B64-4EE5-9F4F-510FBA75D9BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEC00EA-BAE8-433C-ACF9-7C5D94D79DCD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="11" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DriverSheet" sheetId="2" r:id="rId1"/>
@@ -22,12 +22,13 @@
     <sheet name="RealtimeSpineWithNewProperty" sheetId="10" r:id="rId7"/>
     <sheet name="EmailTempWithNewAttribute" sheetId="11" r:id="rId8"/>
     <sheet name="MicrositeTempWithExistingAttrib" sheetId="12" r:id="rId9"/>
-    <sheet name="VerifyDBForNewAgreementModel" sheetId="13" r:id="rId10"/>
-    <sheet name="VerifyAgreementClassFornewProp" sheetId="14" r:id="rId11"/>
-    <sheet name="VerifyDiscardVersioIsSuccessful" sheetId="15" r:id="rId12"/>
-    <sheet name="EnsureRollbackIsSuccessful" sheetId="16" r:id="rId13"/>
-    <sheet name="BatchDecisionOutputValidations" sheetId="8" r:id="rId14"/>
-    <sheet name="CheckLists" sheetId="9" r:id="rId15"/>
+    <sheet name="OBCCTempWithExistingAttrib" sheetId="17" r:id="rId10"/>
+    <sheet name="VerifyDBForNewAgreementModel" sheetId="13" r:id="rId11"/>
+    <sheet name="VerifyAgreementClassFornewProp" sheetId="14" r:id="rId12"/>
+    <sheet name="VerifyDiscardVersioIsSuccessful" sheetId="15" r:id="rId13"/>
+    <sheet name="EnsureRollbackIsSuccessful" sheetId="16" r:id="rId14"/>
+    <sheet name="BatchDecisionOutputValidations" sheetId="8" r:id="rId15"/>
+    <sheet name="CheckLists" sheetId="9" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4661" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4743" uniqueCount="532">
   <si>
     <t>TS1_Regr_01</t>
   </si>
@@ -1475,9 +1476,6 @@
     <t>ADQURA-FW-AppsFW-Data-AgreementStaging</t>
   </si>
   <si>
-    <t>AutoProp</t>
-  </si>
-  <si>
     <t>lnkStagingAgreementClass</t>
   </si>
   <si>
@@ -1626,6 +1624,24 @@
   </si>
   <si>
     <t>PegaGadget5Ifr</t>
+  </si>
+  <si>
+    <t>OBCCTempWithExistingAttrib</t>
+  </si>
+  <si>
+    <t>Verify existing attribute can be added to OBCC template</t>
+  </si>
+  <si>
+    <t>TS15_Regr_01</t>
+  </si>
+  <si>
+    <t>Ensure same attribute added in the email temp can be added to OBCC and verifying in the UI</t>
+  </si>
+  <si>
+    <t>AutoProp1</t>
+  </si>
+  <si>
+    <t>verifying the engine and download</t>
   </si>
 </sst>
 </file>
@@ -2303,10 +2319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK16"/>
+  <dimension ref="A1:AMK17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2513,13 +2529,13 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>482</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>481</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>483</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
@@ -2528,18 +2544,33 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>512</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2552,10 +2583,456 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19DC9284-1E00-457F-9E32-CE2FA20C3859}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="42" t="s">
+        <v>529</v>
+      </c>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="9">
+        <v>5000</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="9">
+        <v>2000</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="9">
+        <v>3000</v>
+      </c>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="F18" s="25"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="D19" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>361</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="25"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>280</v>
+      </c>
+      <c r="F21" s="25">
+        <v>2</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92316FED-85B2-43F2-9827-12AFBA752185}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
@@ -3460,7 +3937,7 @@
         <v>34</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="1"/>
@@ -3543,12 +4020,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDE53E4-1746-48CE-AB4D-617AE971D39B}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3894,7 +4371,7 @@
         <v>63</v>
       </c>
       <c r="F17" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -4204,7 +4681,7 @@
         <v>70</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>476</v>
+        <v>530</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="9"/>
@@ -4451,7 +4928,7 @@
         <v>34</v>
       </c>
       <c r="E44" s="26" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F44" s="25"/>
       <c r="G44" s="1"/>
@@ -4568,18 +5045,20 @@
         <v>462</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>338</v>
+        <v>172</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>472</v>
+        <v>193</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>468</v>
+        <v>34</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="25"/>
+        <v>41</v>
+      </c>
+      <c r="F50" s="25">
+        <v>5000</v>
+      </c>
       <c r="G50" s="25"/>
       <c r="H50" s="25"/>
     </row>
@@ -4588,20 +5067,18 @@
         <v>462</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>64</v>
+        <v>472</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>34</v>
+        <v>468</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="F51" s="25">
-        <v>8000</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F51" s="25"/>
       <c r="G51" s="25"/>
       <c r="H51" s="25"/>
     </row>
@@ -4610,19 +5087,19 @@
         <v>462</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>244</v>
+        <v>64</v>
       </c>
       <c r="D52" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>280</v>
+        <v>41</v>
       </c>
       <c r="F52" s="25">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="G52" s="25"/>
       <c r="H52" s="25"/>
@@ -4632,18 +5109,20 @@
         <v>462</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>473</v>
+        <v>244</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>471</v>
+        <v>34</v>
       </c>
       <c r="E53" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F53" s="25"/>
+        <v>280</v>
+      </c>
+      <c r="F53" s="25">
+        <v>0</v>
+      </c>
       <c r="G53" s="25"/>
       <c r="H53" s="25"/>
     </row>
@@ -4652,20 +5131,18 @@
         <v>462</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C54" s="26" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>34</v>
+        <v>471</v>
       </c>
       <c r="E54" s="26" t="s">
-        <v>469</v>
-      </c>
-      <c r="F54" s="25" t="s">
-        <v>476</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F54" s="25"/>
       <c r="G54" s="25"/>
       <c r="H54" s="25"/>
     </row>
@@ -4677,15 +5154,17 @@
         <v>342</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>185</v>
+        <v>470</v>
       </c>
       <c r="D55" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E55" s="26" t="s">
-        <v>185</v>
-      </c>
-      <c r="F55" s="25"/>
+        <v>469</v>
+      </c>
+      <c r="F55" s="25" t="s">
+        <v>530</v>
+      </c>
       <c r="G55" s="25"/>
       <c r="H55" s="25"/>
     </row>
@@ -4694,20 +5173,18 @@
         <v>462</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="C56" s="25" t="s">
-        <v>467</v>
+        <v>342</v>
+      </c>
+      <c r="C56" s="26" t="s">
+        <v>185</v>
       </c>
       <c r="D56" s="26" t="s">
-        <v>209</v>
+        <v>34</v>
       </c>
       <c r="E56" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="F56" s="37" t="s">
-        <v>475</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="F56" s="25"/>
       <c r="G56" s="25"/>
       <c r="H56" s="25"/>
     </row>
@@ -4716,18 +5193,20 @@
         <v>462</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>344</v>
-      </c>
-      <c r="C57" s="26" t="s">
-        <v>193</v>
+        <v>343</v>
+      </c>
+      <c r="C57" s="25" t="s">
+        <v>467</v>
       </c>
       <c r="D57" s="26" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E57" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F57" s="25"/>
+        <v>70</v>
+      </c>
+      <c r="F57" s="37" t="s">
+        <v>475</v>
+      </c>
       <c r="G57" s="25"/>
       <c r="H57" s="25"/>
     </row>
@@ -4736,13 +5215,13 @@
         <v>462</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C58" s="26" t="s">
-        <v>472</v>
+        <v>193</v>
       </c>
       <c r="D58" s="26" t="s">
-        <v>477</v>
+        <v>212</v>
       </c>
       <c r="E58" s="26" t="s">
         <v>45</v>
@@ -4756,10 +5235,10 @@
         <v>462</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>346</v>
+        <v>172</v>
       </c>
       <c r="C59" s="26" t="s">
-        <v>64</v>
+        <v>193</v>
       </c>
       <c r="D59" s="26" t="s">
         <v>34</v>
@@ -4768,7 +5247,7 @@
         <v>41</v>
       </c>
       <c r="F59" s="25">
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="G59" s="25"/>
       <c r="H59" s="25"/>
@@ -4778,20 +5257,18 @@
         <v>462</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C60" s="26" t="s">
-        <v>244</v>
+        <v>472</v>
       </c>
       <c r="D60" s="26" t="s">
-        <v>34</v>
+        <v>476</v>
       </c>
       <c r="E60" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="F60" s="25">
-        <v>1</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F60" s="25"/>
       <c r="G60" s="25"/>
       <c r="H60" s="25"/>
     </row>
@@ -4800,18 +5277,20 @@
         <v>462</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>384</v>
+        <v>346</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>473</v>
+        <v>64</v>
       </c>
       <c r="D61" s="26" t="s">
-        <v>471</v>
+        <v>34</v>
       </c>
       <c r="E61" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F61" s="25"/>
+        <v>41</v>
+      </c>
+      <c r="F61" s="25">
+        <v>8000</v>
+      </c>
       <c r="G61" s="25"/>
       <c r="H61" s="25"/>
     </row>
@@ -4820,19 +5299,19 @@
         <v>462</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>385</v>
+        <v>346</v>
       </c>
       <c r="C62" s="26" t="s">
-        <v>470</v>
+        <v>244</v>
       </c>
       <c r="D62" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E62" s="26" t="s">
-        <v>469</v>
-      </c>
-      <c r="F62" s="25" t="s">
-        <v>476</v>
+        <v>280</v>
+      </c>
+      <c r="F62" s="25">
+        <v>1</v>
       </c>
       <c r="G62" s="25"/>
       <c r="H62" s="25"/>
@@ -4842,20 +5321,62 @@
         <v>462</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="C63" s="26" t="s">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="D63" s="26" t="s">
-        <v>34</v>
+        <v>471</v>
       </c>
       <c r="E63" s="26" t="s">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="F63" s="25"/>
       <c r="G63" s="25"/>
       <c r="H63" s="25"/>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="A64" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="C64" s="26" t="s">
+        <v>470</v>
+      </c>
+      <c r="D64" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="26" t="s">
+        <v>469</v>
+      </c>
+      <c r="F64" s="25" t="s">
+        <v>530</v>
+      </c>
+      <c r="G64" s="25"/>
+      <c r="H64" s="25"/>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="A65" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>389</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="F65" s="25"/>
+      <c r="G65" s="25"/>
+      <c r="H65" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4868,12 +5389,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D2B88A9-98DC-469F-B6A8-72D4BD0DF47F}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView topLeftCell="C76" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4901,7 +5422,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="42" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
@@ -4949,7 +5470,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>32</v>
@@ -4971,7 +5492,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>36</v>
@@ -4993,7 +5514,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>39</v>
@@ -5015,7 +5536,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>42</v>
@@ -5035,7 +5556,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>46</v>
@@ -5057,7 +5578,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>47</v>
@@ -5077,7 +5598,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>50</v>
@@ -5099,7 +5620,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>51</v>
@@ -5119,7 +5640,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>54</v>
@@ -5141,7 +5662,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>55</v>
@@ -5161,7 +5682,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>58</v>
@@ -5183,7 +5704,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>58</v>
@@ -5205,7 +5726,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>61</v>
@@ -5220,14 +5741,14 @@
         <v>63</v>
       </c>
       <c r="F17" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>61</v>
@@ -5249,7 +5770,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>61</v>
@@ -5269,7 +5790,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>67</v>
@@ -5284,14 +5805,14 @@
         <v>70</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>72</v>
@@ -5306,14 +5827,14 @@
         <v>70</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>76</v>
@@ -5333,7 +5854,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>79</v>
@@ -5355,7 +5876,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>83</v>
@@ -5375,7 +5896,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>89</v>
@@ -5395,7 +5916,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>91</v>
@@ -5415,7 +5936,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>91</v>
@@ -5435,7 +5956,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>93</v>
@@ -5455,7 +5976,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>95</v>
@@ -5475,7 +5996,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>96</v>
@@ -5495,7 +6016,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>97</v>
@@ -5515,7 +6036,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>100</v>
@@ -5524,7 +6045,7 @@
         <v>347</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E32" s="26" t="s">
         <v>45</v>
@@ -5535,7 +6056,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>103</v>
@@ -5550,14 +6071,14 @@
         <v>70</v>
       </c>
       <c r="F33" s="25" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>104</v>
@@ -5577,7 +6098,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>1</v>
@@ -5597,7 +6118,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>108</v>
@@ -5619,7 +6140,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>112</v>
@@ -5639,7 +6160,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>79</v>
@@ -5661,13 +6182,13 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>34</v>
@@ -5676,16 +6197,16 @@
         <v>474</v>
       </c>
       <c r="F39" s="26" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H39" s="9"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>95</v>
@@ -5705,7 +6226,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>96</v>
@@ -5725,7 +6246,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>97</v>
@@ -5740,14 +6261,14 @@
         <v>70</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>100</v>
@@ -5769,7 +6290,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>103</v>
@@ -5784,14 +6305,14 @@
         <v>70</v>
       </c>
       <c r="F44" s="13">
-        <v>45743</v>
+        <v>45719</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="9"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>104</v>
@@ -5811,7 +6332,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>1</v>
@@ -5833,7 +6354,7 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>108</v>
@@ -5853,7 +6374,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>112</v>
@@ -5875,7 +6396,7 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>116</v>
@@ -5895,7 +6416,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>116</v>
@@ -5915,7 +6436,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>119</v>
@@ -5935,7 +6456,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>122</v>
@@ -5955,7 +6476,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>123</v>
@@ -5977,7 +6498,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>156</v>
@@ -5997,7 +6518,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>158</v>
@@ -6019,7 +6540,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>160</v>
@@ -6039,7 +6560,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>160</v>
@@ -6061,7 +6582,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>171</v>
@@ -6073,7 +6594,7 @@
         <v>34</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
@@ -6081,16 +6602,16 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>159</v>
       </c>
       <c r="C59" s="26" t="s">
+        <v>483</v>
+      </c>
+      <c r="D59" s="26" t="s">
         <v>484</v>
-      </c>
-      <c r="D59" s="26" t="s">
-        <v>485</v>
       </c>
       <c r="E59" s="26" t="s">
         <v>452</v>
@@ -6101,7 +6622,7 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>172</v>
@@ -6121,7 +6642,7 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>338</v>
@@ -6143,13 +6664,13 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>339</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>34</v>
@@ -6163,7 +6684,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>340</v>
@@ -6183,13 +6704,13 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>341</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D64" s="9" t="s">
         <v>57</v>
@@ -6203,7 +6724,7 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>341</v>
@@ -6225,7 +6746,7 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>341</v>
@@ -6247,19 +6768,19 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>343</v>
       </c>
       <c r="C67" s="26" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D67" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E67" s="26" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F67" s="25"/>
       <c r="G67" s="25"/>
@@ -6267,13 +6788,13 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>345</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>34</v>
@@ -6289,13 +6810,13 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>346</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>66</v>
@@ -6309,7 +6830,7 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>383</v>
@@ -6324,14 +6845,14 @@
         <v>70</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G70" s="25"/>
       <c r="H70" s="25"/>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>384</v>
@@ -6346,14 +6867,14 @@
         <v>70</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G71" s="25"/>
       <c r="H71" s="25"/>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>385</v>
@@ -6373,7 +6894,7 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>389</v>
@@ -6395,7 +6916,7 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>390</v>
@@ -6415,7 +6936,7 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>395</v>
@@ -6437,7 +6958,7 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>396</v>
@@ -6457,61 +6978,61 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>397</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D77" s="25" t="s">
         <v>34</v>
       </c>
       <c r="E77" s="26" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F77" s="25" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G77" s="37" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H77" s="25"/>
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>398</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D78" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="26" t="s">
+        <v>495</v>
+      </c>
+      <c r="F78" s="26" t="s">
         <v>499</v>
       </c>
-      <c r="D78" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E78" s="26" t="s">
-        <v>496</v>
-      </c>
-      <c r="F78" s="26" t="s">
-        <v>500</v>
-      </c>
       <c r="G78" s="26" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="H78" s="25"/>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>399</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D79" s="38" t="s">
         <v>34</v>
@@ -6527,13 +7048,13 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>400</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D80" s="38" t="s">
         <v>78</v>
@@ -6547,13 +7068,13 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>401</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D81" s="38" t="s">
         <v>34</v>
@@ -6569,13 +7090,13 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>402</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>99</v>
@@ -6589,13 +7110,13 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>403</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>102</v>
@@ -6609,19 +7130,19 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>403</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D84" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F84" s="25"/>
       <c r="G84" s="25"/>
@@ -6629,13 +7150,13 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>403</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D85" s="26" t="s">
         <v>34</v>
@@ -6658,12 +7179,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353D209F-F23A-4BBD-9C0E-30D3275A1C3F}">
   <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B88" workbookViewId="0">
-      <selection activeCell="H99" sqref="H99"/>
+    <sheetView topLeftCell="B76" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6679,7 +7200,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="29.25" customHeight="1">
       <c r="A1" s="44" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B1" s="44"/>
       <c r="C1" s="44"/>
@@ -6737,7 +7258,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>32</v>
@@ -6759,7 +7280,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>36</v>
@@ -6781,7 +7302,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>39</v>
@@ -6803,7 +7324,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>42</v>
@@ -6823,7 +7344,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>46</v>
@@ -6845,7 +7366,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>47</v>
@@ -6865,7 +7386,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>50</v>
@@ -6887,7 +7408,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>51</v>
@@ -6907,7 +7428,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>54</v>
@@ -6929,7 +7450,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>55</v>
@@ -6949,7 +7470,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>58</v>
@@ -6971,7 +7492,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>61</v>
@@ -6993,7 +7514,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>67</v>
@@ -7008,14 +7529,14 @@
         <v>63</v>
       </c>
       <c r="F17" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>72</v>
@@ -7037,7 +7558,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>76</v>
@@ -7057,7 +7578,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>79</v>
@@ -7077,7 +7598,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>83</v>
@@ -7097,7 +7618,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>89</v>
@@ -7117,7 +7638,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>91</v>
@@ -7139,7 +7660,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>93</v>
@@ -7159,7 +7680,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>95</v>
@@ -7174,14 +7695,14 @@
         <v>70</v>
       </c>
       <c r="F25" s="27" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>96</v>
@@ -7201,7 +7722,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>97</v>
@@ -7216,14 +7737,14 @@
         <v>70</v>
       </c>
       <c r="F27" s="30" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>100</v>
@@ -7245,7 +7766,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B29" s="9" t="s">
         <v>103</v>
@@ -7265,7 +7786,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B30" s="9" t="s">
         <v>103</v>
@@ -7285,7 +7806,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B31" s="9" t="s">
         <v>104</v>
@@ -7305,7 +7826,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>1</v>
@@ -7325,7 +7846,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B33" s="9" t="s">
         <v>108</v>
@@ -7347,7 +7868,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>112</v>
@@ -7367,7 +7888,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>116</v>
@@ -7382,14 +7903,14 @@
         <v>70</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G35" s="25"/>
       <c r="H35" s="25"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B36" s="9" t="s">
         <v>119</v>
@@ -7404,14 +7925,14 @@
         <v>70</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G36" s="25"/>
       <c r="H36" s="25"/>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B37" s="9" t="s">
         <v>122</v>
@@ -7431,7 +7952,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B38" s="9" t="s">
         <v>123</v>
@@ -7453,7 +7974,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B39" s="9" t="s">
         <v>156</v>
@@ -7473,7 +7994,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>158</v>
@@ -7493,7 +8014,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B41" s="9" t="s">
         <v>160</v>
@@ -7513,7 +8034,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B42" s="9" t="s">
         <v>171</v>
@@ -7533,7 +8054,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>159</v>
@@ -7553,7 +8074,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>172</v>
@@ -7573,7 +8094,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>338</v>
@@ -7593,7 +8114,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>339</v>
@@ -7613,16 +8134,16 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B47" s="9" t="s">
         <v>340</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E47" s="20" t="s">
         <v>45</v>
@@ -7633,7 +8154,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B48" s="9" t="s">
         <v>341</v>
@@ -7648,14 +8169,14 @@
         <v>70</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G48" s="25"/>
       <c r="H48" s="25"/>
     </row>
     <row r="49" spans="1:8">
       <c r="A49" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B49" s="9" t="s">
         <v>342</v>
@@ -7675,7 +8196,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B50" s="9" t="s">
         <v>343</v>
@@ -7695,7 +8216,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>344</v>
@@ -7717,7 +8238,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>340</v>
@@ -7737,7 +8258,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>341</v>
@@ -7759,7 +8280,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>342</v>
@@ -7779,7 +8300,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>343</v>
@@ -7799,7 +8320,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>344</v>
@@ -7814,14 +8335,14 @@
         <v>70</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G56" s="25"/>
       <c r="H56" s="25"/>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>345</v>
@@ -7843,7 +8364,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B58" s="9" t="s">
         <v>346</v>
@@ -7858,14 +8379,14 @@
         <v>70</v>
       </c>
       <c r="F58" s="13">
-        <v>45743</v>
+        <v>45717</v>
       </c>
       <c r="G58" s="25"/>
       <c r="H58" s="25"/>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B59" s="9" t="s">
         <v>383</v>
@@ -7885,7 +8406,7 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B60" s="36" t="s">
         <v>383</v>
@@ -7907,7 +8428,7 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B61" s="36" t="s">
         <v>384</v>
@@ -7927,7 +8448,7 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B62" s="36" t="s">
         <v>384</v>
@@ -7949,7 +8470,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B63" s="36" t="s">
         <v>384</v>
@@ -7969,7 +8490,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B64" s="36" t="s">
         <v>384</v>
@@ -7989,7 +8510,7 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>385</v>
@@ -8004,14 +8525,14 @@
         <v>149</v>
       </c>
       <c r="F65" s="29" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G65" s="25"/>
       <c r="H65" s="25"/>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>389</v>
@@ -8026,14 +8547,14 @@
         <v>394</v>
       </c>
       <c r="F66" s="27" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G66" s="25"/>
       <c r="H66" s="25"/>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B67" s="9" t="s">
         <v>390</v>
@@ -8055,7 +8576,7 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>395</v>
@@ -8075,7 +8596,7 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>396</v>
@@ -8097,7 +8618,7 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B70" s="9" t="s">
         <v>397</v>
@@ -8117,7 +8638,7 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B71" s="9" t="s">
         <v>398</v>
@@ -8139,7 +8660,7 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>399</v>
@@ -8159,7 +8680,7 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B73" s="9" t="s">
         <v>400</v>
@@ -8179,7 +8700,7 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B74" s="9" t="s">
         <v>400</v>
@@ -8191,7 +8712,7 @@
         <v>34</v>
       </c>
       <c r="E74" s="26" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F74" s="1"/>
       <c r="G74" s="25"/>
@@ -8199,11 +8720,11 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B75" s="9"/>
       <c r="C75" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>34</v>
@@ -8212,22 +8733,22 @@
         <v>474</v>
       </c>
       <c r="F75" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="G75" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>521</v>
       </c>
       <c r="H75" s="25"/>
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B76" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>34</v>
@@ -8241,7 +8762,7 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B77" s="9" t="s">
         <v>400</v>
@@ -8261,13 +8782,13 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B78" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D78" s="9" t="s">
         <v>57</v>
@@ -8281,7 +8802,7 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>400</v>
@@ -8303,7 +8824,7 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>400</v>
@@ -8318,20 +8839,20 @@
         <v>59</v>
       </c>
       <c r="F80" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G80" s="25"/>
       <c r="H80" s="25"/>
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C81" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>34</v>
@@ -8347,7 +8868,7 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B82" s="9" t="s">
         <v>400</v>
@@ -8362,14 +8883,14 @@
         <v>63</v>
       </c>
       <c r="F82" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G82" s="25"/>
       <c r="H82" s="25"/>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B83" s="9" t="s">
         <v>400</v>
@@ -8391,16 +8912,16 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B84" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C84" s="27" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E84" s="25" t="s">
         <v>45</v>
@@ -8411,7 +8932,7 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B85" s="9" t="s">
         <v>400</v>
@@ -8431,13 +8952,13 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B86" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C86" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>34</v>
@@ -8453,13 +8974,13 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B87" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C87" s="25" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>78</v>
@@ -8473,13 +8994,13 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B88" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C88" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>34</v>
@@ -8495,13 +9016,13 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B89" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C89" s="25" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>78</v>
@@ -8515,13 +9036,13 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B90" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C90" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>34</v>
@@ -8537,61 +9058,61 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B91" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C91" s="25" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D91" s="25" t="s">
         <v>34</v>
       </c>
       <c r="E91" s="26" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F91" s="25" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G91" s="25" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H91" s="25"/>
     </row>
     <row r="92" spans="1:8">
       <c r="A92" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D92" s="25" t="s">
         <v>34</v>
       </c>
       <c r="E92" s="26" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F92" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="G92" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>521</v>
       </c>
       <c r="H92" s="25"/>
     </row>
     <row r="93" spans="1:8">
       <c r="A93" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B93" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C93" s="25" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>78</v>
@@ -8605,7 +9126,7 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>400</v>
@@ -8627,13 +9148,13 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>34</v>
@@ -8647,7 +9168,7 @@
     </row>
     <row r="96" spans="1:8">
       <c r="A96" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B96" s="9" t="s">
         <v>400</v>
@@ -8667,13 +9188,13 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B97" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C97" s="25" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>57</v>
@@ -8687,7 +9208,7 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B98" s="9" t="s">
         <v>400</v>
@@ -8709,7 +9230,7 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B99" s="9" t="s">
         <v>400</v>
@@ -8724,20 +9245,20 @@
         <v>59</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G99" s="25"/>
       <c r="H99" s="25"/>
     </row>
     <row r="100" spans="1:8">
       <c r="A100" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B100" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C100" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>34</v>
@@ -8753,29 +9274,29 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B101" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C101" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D101" s="26" t="s">
         <v>34</v>
       </c>
       <c r="E101" s="27" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F101" s="25" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G101" s="25"/>
       <c r="H101" s="25"/>
     </row>
     <row r="102" spans="1:8">
       <c r="A102" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B102" s="9" t="s">
         <v>400</v>
@@ -8797,16 +9318,16 @@
     </row>
     <row r="103" spans="1:8">
       <c r="A103" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B103" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C103" s="27" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D103" s="26" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E103" s="25" t="s">
         <v>45</v>
@@ -8817,7 +9338,7 @@
     </row>
     <row r="104" spans="1:8">
       <c r="A104" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B104" s="9" t="s">
         <v>400</v>
@@ -8837,13 +9358,13 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B105" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C105" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>34</v>
@@ -8859,13 +9380,13 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B106" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C106" s="25" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>78</v>
@@ -8879,13 +9400,13 @@
     </row>
     <row r="107" spans="1:8">
       <c r="A107" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B107" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C107" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>34</v>
@@ -8901,13 +9422,13 @@
     </row>
     <row r="108" spans="1:8">
       <c r="A108" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B108" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C108" s="25" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>78</v>
@@ -8921,13 +9442,13 @@
     </row>
     <row r="109" spans="1:8">
       <c r="A109" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B109" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C109" s="25" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>34</v>
@@ -8943,37 +9464,37 @@
     </row>
     <row r="110" spans="1:8">
       <c r="A110" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B110" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C110" s="25" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D110" s="25" t="s">
         <v>34</v>
       </c>
       <c r="E110" s="26" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F110" s="25" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G110" s="37" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="H110" s="25"/>
     </row>
     <row r="111" spans="1:8">
       <c r="A111" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B111" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D111" s="25" t="s">
         <v>34</v>
@@ -8982,22 +9503,22 @@
         <v>474</v>
       </c>
       <c r="F111" s="26" t="s">
+        <v>519</v>
+      </c>
+      <c r="G111" s="1" t="s">
         <v>520</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>521</v>
       </c>
       <c r="H111" s="25"/>
     </row>
     <row r="112" spans="1:8">
       <c r="A112" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B112" s="9" t="s">
         <v>400</v>
       </c>
       <c r="C112" s="25" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>78</v>
@@ -9011,7 +9532,7 @@
     </row>
     <row r="113" spans="1:8">
       <c r="A113" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B113" s="9" t="s">
         <v>400</v>
@@ -9033,7 +9554,7 @@
     </row>
     <row r="114" spans="1:8">
       <c r="A114" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="B114" s="9" t="s">
         <v>400</v>
@@ -9062,7 +9583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -9250,7 +9771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:B3"/>
   <sheetViews>
@@ -9289,10 +9810,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39:F39"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9640,7 +10161,7 @@
         <v>63</v>
       </c>
       <c r="F17" s="9">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="1"/>
@@ -10148,16 +10669,16 @@
         <v>0</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>105</v>
+        <v>531</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>106</v>
+        <v>34</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -10168,144 +10689,20 @@
         <v>0</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E43" s="12" t="s">
-        <v>111</v>
+        <v>34</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>125</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F45" s="1">
-        <v>10000</v>
-      </c>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" s="1">
-        <v>30000</v>
-      </c>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10322,8 +10719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10670,7 +11067,7 @@
         <v>63</v>
       </c>
       <c r="F17" s="9">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
@@ -10725,13 +11122,13 @@
         <v>61</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D20" s="20" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -11126,7 +11523,7 @@
         <v>70</v>
       </c>
       <c r="F39" s="13">
-        <v>45743</v>
+        <v>45719</v>
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="9"/>
@@ -11727,7 +12124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -12840,8 +13237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H85"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13883,7 +14280,7 @@
         <v>70</v>
       </c>
       <c r="F50" s="13">
-        <v>45743</v>
+        <v>45717</v>
       </c>
       <c r="G50" s="13"/>
       <c r="H50" s="9"/>
@@ -14645,7 +15042,7 @@
   </sheetPr>
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -16377,7 +16774,7 @@
   </sheetPr>
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0">
+    <sheetView topLeftCell="A91" workbookViewId="0">
       <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
@@ -18458,8 +18855,8 @@
   </sheetPr>
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19551,7 +19948,7 @@
         <v>70</v>
       </c>
       <c r="F53" s="13">
-        <v>45743</v>
+        <v>45719</v>
       </c>
       <c r="G53" s="25"/>
       <c r="H53" s="25"/>
@@ -20053,8 +20450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10CE6C41-C6E4-4D12-92D1-A13E0879FD5B}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="J70" sqref="J70"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21144,7 +21541,7 @@
         <v>70</v>
       </c>
       <c r="F53" s="13">
-        <v>45743</v>
+        <v>45719</v>
       </c>
       <c r="G53" s="25"/>
       <c r="H53" s="25"/>

</xml_diff>

<commit_message>
rerunning the failed cases
</commit_message>
<xml_diff>
--- a/TestDataAndResults/TestData/SophieAutomation.xlsx
+++ b/TestDataAndResults/TestData/SophieAutomation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deepa\eclipse-workspace\SofieKDF_HeadLess_5819_V2\SofieKDF_HeadLess_5819\SofieKDFHeadless\TestDataAndResults\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA17C2A4-664A-4977-BC18-B2F33E4E1F89}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A73D0F-4F99-44DC-8366-0189705E140A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" firstSheet="16" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DriverSheet" sheetId="2" r:id="rId1"/>
@@ -2531,8 +2531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2598,7 +2598,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>591</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -2613,7 +2613,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>591</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -2643,7 +2643,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>591</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -2733,7 +2733,7 @@
         <v>464</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
+        <v>591</v>
       </c>
       <c r="E14" s="1"/>
     </row>
@@ -2793,7 +2793,7 @@
         <v>547</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>591</v>
       </c>
       <c r="E18" s="1"/>
     </row>
@@ -6155,8 +6155,8 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13610,8 +13610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB81825B-AC84-43BA-896B-AD045DB7862F}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>